<commit_message>
complete sent notification admin side
</commit_message>
<xml_diff>
--- a/downloads/exported_data.xlsx
+++ b/downloads/exported_data.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,24 +422,75 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>Jignesh</v>
+      </c>
+      <c r="B2" t="str">
+        <v>jignesh1234@gmail.com</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45390.771060914354</v>
+      </c>
+      <c r="D2" t="str">
+        <v>18:29:2</v>
+      </c>
+      <c r="E2" t="str">
+        <v>18:30:5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
         <v>parth</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B3" t="str">
         <v>parthpatel082828@gmail.com</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="1">
+        <v>45390.77028099537</v>
+      </c>
+      <c r="D3" t="str">
+        <v>18:27:0</v>
+      </c>
+      <c r="E3" t="str">
+        <v>18:28:23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Jignesh</v>
+      </c>
+      <c r="B4" t="str">
+        <v>jignesh1234@gmail.com</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45390.76887056713</v>
+      </c>
+      <c r="D4" t="str">
+        <v>18:26:42</v>
+      </c>
+      <c r="E4" t="str">
+        <v>18:26:49</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B5" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C5" s="1">
         <v>45387.22928240741</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D5" t="str">
         <v>02:53 PM</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E5" t="str">
         <v>02:54 PM</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add cart functionality in process
</commit_message>
<xml_diff>
--- a/downloads/exported_data.xlsx
+++ b/downloads/exported_data.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,75 +422,92 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Jignesh</v>
+        <v>parth</v>
       </c>
       <c r="B2" t="str">
-        <v>jignesh1234@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C2" s="1">
-        <v>45390.771060914354</v>
+        <v>45406.67672707176</v>
       </c>
       <c r="D2" t="str">
-        <v>18:29:2</v>
+        <v>15:52:4</v>
       </c>
       <c r="E2" t="str">
-        <v>18:30:5</v>
+        <v>16:12:36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>parth</v>
+        <v>Jignesh</v>
       </c>
       <c r="B3" t="str">
-        <v>parthpatel082828@gmail.com</v>
+        <v>jignesh1234@gmail.com</v>
       </c>
       <c r="C3" s="1">
-        <v>45390.77028099537</v>
+        <v>45390.771060914354</v>
       </c>
       <c r="D3" t="str">
-        <v>18:27:0</v>
+        <v>18:29:2</v>
       </c>
       <c r="E3" t="str">
-        <v>18:28:23</v>
+        <v>18:30:5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Jignesh</v>
+        <v>parth</v>
       </c>
       <c r="B4" t="str">
-        <v>jignesh1234@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C4" s="1">
-        <v>45390.76887056713</v>
+        <v>45390.77028099537</v>
       </c>
       <c r="D4" t="str">
-        <v>18:26:42</v>
+        <v>18:27:0</v>
       </c>
       <c r="E4" t="str">
-        <v>18:26:49</v>
+        <v>18:28:23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
+        <v>Jignesh</v>
+      </c>
+      <c r="B5" t="str">
+        <v>jignesh1234@gmail.com</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45390.76887056713</v>
+      </c>
+      <c r="D5" t="str">
+        <v>18:26:42</v>
+      </c>
+      <c r="E5" t="str">
+        <v>18:26:49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
         <v>parth</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B6" t="str">
         <v>parthpatel082828@gmail.com</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>45387.22928240741</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D6" t="str">
         <v>02:53 PM</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E6" t="str">
         <v>02:54 PM</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit address issue solve at time of placeorder and admin can't change the user password
</commit_message>
<xml_diff>
--- a/downloads/exported_data.xlsx
+++ b/downloads/exported_data.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,30 +428,30 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C2" s="1">
-        <v>45406.67672707176</v>
+        <v>45427.42300994213</v>
       </c>
       <c r="D2" t="str">
-        <v>15:52:4</v>
+        <v>10:8:47</v>
       </c>
       <c r="E2" t="str">
-        <v>16:12:36</v>
+        <v>10:8:53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Jignesh</v>
+        <v>parth</v>
       </c>
       <c r="B3" t="str">
-        <v>jignesh1234@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C3" s="1">
-        <v>45390.771060914354</v>
+        <v>45427.42250050926</v>
       </c>
       <c r="D3" t="str">
-        <v>18:29:2</v>
+        <v>10:7:57</v>
       </c>
       <c r="E3" t="str">
-        <v>18:30:5</v>
+        <v>10:8:6</v>
       </c>
     </row>
     <row r="4">
@@ -462,30 +462,30 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C4" s="1">
-        <v>45390.77028099537</v>
+        <v>45427.42184621528</v>
       </c>
       <c r="D4" t="str">
-        <v>18:27:0</v>
+        <v>10:7:3</v>
       </c>
       <c r="E4" t="str">
-        <v>18:28:23</v>
+        <v>10:7:12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Jignesh</v>
+        <v>parth</v>
       </c>
       <c r="B5" t="str">
-        <v>jignesh1234@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C5" s="1">
-        <v>45390.76887056713</v>
+        <v>45427.42166769676</v>
       </c>
       <c r="D5" t="str">
-        <v>18:26:42</v>
+        <v>9:52:49</v>
       </c>
       <c r="E5" t="str">
-        <v>18:26:49</v>
+        <v>10:6:55</v>
       </c>
     </row>
     <row r="6">
@@ -496,18 +496,613 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C6" s="1">
+        <v>45427.41121439815</v>
+      </c>
+      <c r="D6" t="str">
+        <v>9:43:10</v>
+      </c>
+      <c r="E6" t="str">
+        <v>9:51:55</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B7" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45427.39575678241</v>
+      </c>
+      <c r="D7" t="str">
+        <v>9:29:27</v>
+      </c>
+      <c r="E7" t="str">
+        <v>9:29:38</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B8" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45424.862643333334</v>
+      </c>
+      <c r="D8" t="str">
+        <v>17:11:1</v>
+      </c>
+      <c r="E8" t="str">
+        <v>18:10:21</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B9" t="str">
+        <v>patelparth682841@gmail.com</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45420.47029642361</v>
+      </c>
+      <c r="D9" t="str">
+        <v>20:18:27</v>
+      </c>
+      <c r="E9" t="str">
+        <v>10:36:56</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Harita</v>
+      </c>
+      <c r="B10" t="str">
+        <v>hdumradiya.weapplinse@gmail.com</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45419.7901571875</v>
+      </c>
+      <c r="D10" t="str">
+        <v>18:47:36</v>
+      </c>
+      <c r="E10" t="str">
+        <v>18:57:1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>vatsal</v>
+      </c>
+      <c r="B11" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45419.66625256944</v>
+      </c>
+      <c r="D11" t="str">
+        <v>12:36:3</v>
+      </c>
+      <c r="E11" t="str">
+        <v>15:59:9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B12" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C12" s="1">
         <v>45387.22928240741</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D12" t="str">
         <v>02:53 PM</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E12" t="str">
+        <v>02:54 PM</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Jignesh</v>
+      </c>
+      <c r="B13" t="str">
+        <v>jignesh1234@gmail.com</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45390.76886574074</v>
+      </c>
+      <c r="D13" t="str">
+        <v>18:26:42</v>
+      </c>
+      <c r="E13" t="str">
+        <v>18:26:49</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B14" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45390.77027777778</v>
+      </c>
+      <c r="D14" t="str">
+        <v>18:27:0</v>
+      </c>
+      <c r="E14" t="str">
+        <v>18:28:23</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Jignesh</v>
+      </c>
+      <c r="B15" t="str">
+        <v>jignesh1234@gmail.com</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45390.771053240744</v>
+      </c>
+      <c r="D15" t="str">
+        <v>18:29:2</v>
+      </c>
+      <c r="E15" t="str">
+        <v>18:30:5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B16" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45406.676724537036</v>
+      </c>
+      <c r="D16" t="str">
+        <v>15:52:4</v>
+      </c>
+      <c r="E16" t="str">
+        <v>16:12:36</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B17" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45411.70990740741</v>
+      </c>
+      <c r="D17" t="str">
+        <v>17:1:31</v>
+      </c>
+      <c r="E17" t="str">
+        <v>17:1:57</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B18" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45411.74334490741</v>
+      </c>
+      <c r="D18" t="str">
+        <v>17:2:6</v>
+      </c>
+      <c r="E18" t="str">
+        <v>17:50:11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B19" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45413.74621527778</v>
+      </c>
+      <c r="D19" t="str">
+        <v>17:52:23</v>
+      </c>
+      <c r="E19" t="str">
+        <v>17:54:17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B20" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45413.75671296296</v>
+      </c>
+      <c r="D20" t="str">
+        <v>17:54:23</v>
+      </c>
+      <c r="E20" t="str">
+        <v>18:7:23</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B21" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45414.39465277778</v>
+      </c>
+      <c r="D21" t="str">
+        <v>9:27:54</v>
+      </c>
+      <c r="E21" t="str">
+        <v>9:28:5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B22" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C22" s="1">
+        <v>45414.39488425926</v>
+      </c>
+      <c r="D22" t="str">
+        <v>9:28:8</v>
+      </c>
+      <c r="E22" t="str">
+        <v>9:28:25</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B23" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C23" s="1">
+        <v>45414.39942129629</v>
+      </c>
+      <c r="D23" t="str">
+        <v>9:34:34</v>
+      </c>
+      <c r="E23" t="str">
+        <v>9:34:41</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>test</v>
+      </c>
+      <c r="B24" t="str">
+        <v>test@gmail.com</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45415.510625</v>
+      </c>
+      <c r="D24" t="str">
+        <v>12:5:48</v>
+      </c>
+      <c r="E24" t="str">
+        <v>12:15:2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>avi</v>
+      </c>
+      <c r="B25" t="str">
+        <v>avi@gmail.com</v>
+      </c>
+      <c r="C25" s="1">
+        <v>45416.360497685186</v>
+      </c>
+      <c r="D25" t="str">
+        <v>8:37:40</v>
+      </c>
+      <c r="E25" t="str">
+        <v>8:38:44</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>vatsal</v>
+      </c>
+      <c r="B26" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45416.84626157407</v>
+      </c>
+      <c r="D26" t="str">
+        <v>14:9:6</v>
+      </c>
+      <c r="E26" t="str">
+        <v>20:18:15</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>vatsal</v>
+      </c>
+      <c r="B27" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C27" s="1">
+        <v>45416.846269837966</v>
+      </c>
+      <c r="D27" t="str">
+        <v>14:9:6</v>
+      </c>
+      <c r="E27" t="str">
+        <v>20:18:15</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>avi</v>
+      </c>
+      <c r="B28" t="str">
+        <v>avi@gmail.com</v>
+      </c>
+      <c r="C28" s="1">
+        <v>45416.360501296294</v>
+      </c>
+      <c r="D28" t="str">
+        <v>8:37:40</v>
+      </c>
+      <c r="E28" t="str">
+        <v>8:38:44</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>test</v>
+      </c>
+      <c r="B29" t="str">
+        <v>test@gmail.com</v>
+      </c>
+      <c r="C29" s="1">
+        <v>45415.51063256944</v>
+      </c>
+      <c r="D29" t="str">
+        <v>12:5:48</v>
+      </c>
+      <c r="E29" t="str">
+        <v>12:15:2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B30" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C30" s="1">
+        <v>45414.399427777775</v>
+      </c>
+      <c r="D30" t="str">
+        <v>9:34:34</v>
+      </c>
+      <c r="E30" t="str">
+        <v>9:34:41</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B31" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C31" s="1">
+        <v>45414.39488688658</v>
+      </c>
+      <c r="D31" t="str">
+        <v>9:28:8</v>
+      </c>
+      <c r="E31" t="str">
+        <v>9:28:25</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B32" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C32" s="1">
+        <v>45414.39466230324</v>
+      </c>
+      <c r="D32" t="str">
+        <v>9:27:54</v>
+      </c>
+      <c r="E32" t="str">
+        <v>9:28:5</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B33" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C33" s="1">
+        <v>45413.75671300926</v>
+      </c>
+      <c r="D33" t="str">
+        <v>17:54:23</v>
+      </c>
+      <c r="E33" t="str">
+        <v>18:7:23</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B34" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C34" s="1">
+        <v>45413.74621600694</v>
+      </c>
+      <c r="D34" t="str">
+        <v>17:52:23</v>
+      </c>
+      <c r="E34" t="str">
+        <v>17:54:17</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B35" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C35" s="1">
+        <v>45411.74335091435</v>
+      </c>
+      <c r="D35" t="str">
+        <v>17:2:6</v>
+      </c>
+      <c r="E35" t="str">
+        <v>17:50:11</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B36" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C36" s="1">
+        <v>45411.70991153935</v>
+      </c>
+      <c r="D36" t="str">
+        <v>17:1:31</v>
+      </c>
+      <c r="E36" t="str">
+        <v>17:1:57</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B37" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C37" s="1">
+        <v>45406.67672707176</v>
+      </c>
+      <c r="D37" t="str">
+        <v>15:52:4</v>
+      </c>
+      <c r="E37" t="str">
+        <v>16:12:36</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Jignesh</v>
+      </c>
+      <c r="B38" t="str">
+        <v>jignesh1234@gmail.com</v>
+      </c>
+      <c r="C38" s="1">
+        <v>45390.771060914354</v>
+      </c>
+      <c r="D38" t="str">
+        <v>18:29:2</v>
+      </c>
+      <c r="E38" t="str">
+        <v>18:30:5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B39" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C39" s="1">
+        <v>45390.77028099537</v>
+      </c>
+      <c r="D39" t="str">
+        <v>18:27:0</v>
+      </c>
+      <c r="E39" t="str">
+        <v>18:28:23</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Jignesh</v>
+      </c>
+      <c r="B40" t="str">
+        <v>jignesh1234@gmail.com</v>
+      </c>
+      <c r="C40" s="1">
+        <v>45390.76887056713</v>
+      </c>
+      <c r="D40" t="str">
+        <v>18:26:42</v>
+      </c>
+      <c r="E40" t="str">
+        <v>18:26:49</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B41" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C41" s="1">
+        <v>45387.22928240741</v>
+      </c>
+      <c r="D41" t="str">
+        <v>02:53 PM</v>
+      </c>
+      <c r="E41" t="str">
         <v>02:54 PM</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E41"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
order managment both side is completed
</commit_message>
<xml_diff>
--- a/downloads/exported_data.xlsx
+++ b/downloads/exported_data.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,13 +428,13 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C2" s="1">
-        <v>45427.42300994213</v>
+        <v>45432.82773920139</v>
       </c>
       <c r="D2" t="str">
-        <v>10:8:47</v>
+        <v>16:55:21</v>
       </c>
       <c r="E2" t="str">
-        <v>10:8:53</v>
+        <v>19:51:46</v>
       </c>
     </row>
     <row r="3">
@@ -445,13 +445,13 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C3" s="1">
-        <v>45427.42250050926</v>
+        <v>45429.42889310185</v>
       </c>
       <c r="D3" t="str">
-        <v>10:7:57</v>
+        <v>10:16:54</v>
       </c>
       <c r="E3" t="str">
-        <v>10:8:6</v>
+        <v>10:17:26</v>
       </c>
     </row>
     <row r="4">
@@ -462,13 +462,13 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C4" s="1">
-        <v>45427.42184621528</v>
+        <v>45429.425747361114</v>
       </c>
       <c r="D4" t="str">
-        <v>10:7:3</v>
+        <v>10:12:34</v>
       </c>
       <c r="E4" t="str">
-        <v>10:7:12</v>
+        <v>10:12:50</v>
       </c>
     </row>
     <row r="5">
@@ -479,13 +479,13 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C5" s="1">
-        <v>45427.42166769676</v>
+        <v>45429.425500335645</v>
       </c>
       <c r="D5" t="str">
-        <v>9:52:49</v>
+        <v>10:12:18</v>
       </c>
       <c r="E5" t="str">
-        <v>10:6:55</v>
+        <v>10:12:28</v>
       </c>
     </row>
     <row r="6">
@@ -496,30 +496,30 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C6" s="1">
-        <v>45427.41121439815</v>
+        <v>45429.4253</v>
       </c>
       <c r="D6" t="str">
-        <v>9:43:10</v>
+        <v>14:11:47</v>
       </c>
       <c r="E6" t="str">
-        <v>9:51:55</v>
+        <v>10:12:11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>parth</v>
+        <v>mical</v>
       </c>
       <c r="B7" t="str">
-        <v>parthpatel082828@gmail.com</v>
+        <v>madibic334@nweal.com</v>
       </c>
       <c r="C7" s="1">
-        <v>45427.39575678241</v>
+        <v>45428.78524579861</v>
       </c>
       <c r="D7" t="str">
-        <v>9:29:27</v>
+        <v>18:49:4</v>
       </c>
       <c r="E7" t="str">
-        <v>9:29:38</v>
+        <v>18:49:49</v>
       </c>
     </row>
     <row r="8">
@@ -530,13 +530,13 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C8" s="1">
-        <v>45424.862643333334</v>
+        <v>45427.591582546294</v>
       </c>
       <c r="D8" t="str">
-        <v>17:11:1</v>
+        <v>10:9:1</v>
       </c>
       <c r="E8" t="str">
-        <v>18:10:21</v>
+        <v>14:11:38</v>
       </c>
     </row>
     <row r="9">
@@ -544,50 +544,50 @@
         <v>parth</v>
       </c>
       <c r="B9" t="str">
-        <v>patelparth682841@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C9" s="1">
-        <v>45420.47029642361</v>
+        <v>45427.42300994213</v>
       </c>
       <c r="D9" t="str">
-        <v>20:18:27</v>
+        <v>10:8:47</v>
       </c>
       <c r="E9" t="str">
-        <v>10:36:56</v>
+        <v>10:8:53</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Harita</v>
+        <v>parth</v>
       </c>
       <c r="B10" t="str">
-        <v>hdumradiya.weapplinse@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C10" s="1">
-        <v>45419.7901571875</v>
+        <v>45427.42250050926</v>
       </c>
       <c r="D10" t="str">
-        <v>18:47:36</v>
+        <v>10:7:57</v>
       </c>
       <c r="E10" t="str">
-        <v>18:57:1</v>
+        <v>10:8:6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>vatsal</v>
+        <v>parth</v>
       </c>
       <c r="B11" t="str">
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C11" s="1">
-        <v>45419.66625256944</v>
+        <v>45427.42184621528</v>
       </c>
       <c r="D11" t="str">
-        <v>12:36:3</v>
+        <v>10:7:3</v>
       </c>
       <c r="E11" t="str">
-        <v>15:59:9</v>
+        <v>10:7:12</v>
       </c>
     </row>
     <row r="12">
@@ -598,30 +598,30 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C12" s="1">
-        <v>45387.22928240741</v>
+        <v>45427.42166769676</v>
       </c>
       <c r="D12" t="str">
-        <v>02:53 PM</v>
+        <v>9:52:49</v>
       </c>
       <c r="E12" t="str">
-        <v>02:54 PM</v>
+        <v>10:6:55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Jignesh</v>
+        <v>parth</v>
       </c>
       <c r="B13" t="str">
-        <v>jignesh1234@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C13" s="1">
-        <v>45390.76886574074</v>
+        <v>45427.41121439815</v>
       </c>
       <c r="D13" t="str">
-        <v>18:26:42</v>
+        <v>9:43:10</v>
       </c>
       <c r="E13" t="str">
-        <v>18:26:49</v>
+        <v>9:51:55</v>
       </c>
     </row>
     <row r="14">
@@ -632,30 +632,30 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C14" s="1">
-        <v>45390.77027777778</v>
+        <v>45427.39575678241</v>
       </c>
       <c r="D14" t="str">
-        <v>18:27:0</v>
+        <v>9:29:27</v>
       </c>
       <c r="E14" t="str">
-        <v>18:28:23</v>
+        <v>9:29:38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Jignesh</v>
+        <v>parth</v>
       </c>
       <c r="B15" t="str">
-        <v>jignesh1234@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C15" s="1">
-        <v>45390.771053240744</v>
+        <v>45424.862643333334</v>
       </c>
       <c r="D15" t="str">
-        <v>18:29:2</v>
+        <v>17:11:1</v>
       </c>
       <c r="E15" t="str">
-        <v>18:30:5</v>
+        <v>18:10:21</v>
       </c>
     </row>
     <row r="16">
@@ -663,50 +663,50 @@
         <v>parth</v>
       </c>
       <c r="B16" t="str">
-        <v>parthpatel082828@gmail.com</v>
+        <v>patelparth682841@gmail.com</v>
       </c>
       <c r="C16" s="1">
-        <v>45406.676724537036</v>
+        <v>45420.47029642361</v>
       </c>
       <c r="D16" t="str">
-        <v>15:52:4</v>
+        <v>20:18:27</v>
       </c>
       <c r="E16" t="str">
-        <v>16:12:36</v>
+        <v>10:36:56</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>parth</v>
+        <v>Harita</v>
       </c>
       <c r="B17" t="str">
-        <v>parthpatel082828@gmail.com</v>
+        <v>hdumradiya.weapplinse@gmail.com</v>
       </c>
       <c r="C17" s="1">
-        <v>45411.70990740741</v>
+        <v>45419.7901571875</v>
       </c>
       <c r="D17" t="str">
-        <v>17:1:31</v>
+        <v>18:47:36</v>
       </c>
       <c r="E17" t="str">
-        <v>17:1:57</v>
+        <v>18:57:1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>parth</v>
+        <v>vatsal</v>
       </c>
       <c r="B18" t="str">
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C18" s="1">
-        <v>45411.74334490741</v>
+        <v>45419.66625256944</v>
       </c>
       <c r="D18" t="str">
-        <v>17:2:6</v>
+        <v>12:36:3</v>
       </c>
       <c r="E18" t="str">
-        <v>17:50:11</v>
+        <v>15:59:9</v>
       </c>
     </row>
     <row r="19">
@@ -717,30 +717,30 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C19" s="1">
-        <v>45413.74621527778</v>
+        <v>45387.22928240741</v>
       </c>
       <c r="D19" t="str">
-        <v>17:52:23</v>
+        <v>02:53 PM</v>
       </c>
       <c r="E19" t="str">
-        <v>17:54:17</v>
+        <v>02:54 PM</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>parth</v>
+        <v>Jignesh</v>
       </c>
       <c r="B20" t="str">
-        <v>parthpatel082828@gmail.com</v>
+        <v>jignesh1234@gmail.com</v>
       </c>
       <c r="C20" s="1">
-        <v>45413.75671296296</v>
+        <v>45390.76886574074</v>
       </c>
       <c r="D20" t="str">
-        <v>17:54:23</v>
+        <v>18:26:42</v>
       </c>
       <c r="E20" t="str">
-        <v>18:7:23</v>
+        <v>18:26:49</v>
       </c>
     </row>
     <row r="21">
@@ -751,30 +751,30 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C21" s="1">
-        <v>45414.39465277778</v>
+        <v>45390.77027777778</v>
       </c>
       <c r="D21" t="str">
-        <v>9:27:54</v>
+        <v>18:27:0</v>
       </c>
       <c r="E21" t="str">
-        <v>9:28:5</v>
+        <v>18:28:23</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>parth</v>
+        <v>Jignesh</v>
       </c>
       <c r="B22" t="str">
-        <v>parthpatel082828@gmail.com</v>
+        <v>jignesh1234@gmail.com</v>
       </c>
       <c r="C22" s="1">
-        <v>45414.39488425926</v>
+        <v>45390.771053240744</v>
       </c>
       <c r="D22" t="str">
-        <v>9:28:8</v>
+        <v>18:29:2</v>
       </c>
       <c r="E22" t="str">
-        <v>9:28:25</v>
+        <v>18:30:5</v>
       </c>
     </row>
     <row r="23">
@@ -785,115 +785,115 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C23" s="1">
-        <v>45414.39942129629</v>
+        <v>45406.676724537036</v>
       </c>
       <c r="D23" t="str">
-        <v>9:34:34</v>
+        <v>15:52:4</v>
       </c>
       <c r="E23" t="str">
-        <v>9:34:41</v>
+        <v>16:12:36</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>test</v>
+        <v>parth</v>
       </c>
       <c r="B24" t="str">
-        <v>test@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C24" s="1">
-        <v>45415.510625</v>
+        <v>45411.70990740741</v>
       </c>
       <c r="D24" t="str">
-        <v>12:5:48</v>
+        <v>17:1:31</v>
       </c>
       <c r="E24" t="str">
-        <v>12:15:2</v>
+        <v>17:1:57</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>avi</v>
+        <v>parth</v>
       </c>
       <c r="B25" t="str">
-        <v>avi@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C25" s="1">
-        <v>45416.360497685186</v>
+        <v>45411.74334490741</v>
       </c>
       <c r="D25" t="str">
-        <v>8:37:40</v>
+        <v>17:2:6</v>
       </c>
       <c r="E25" t="str">
-        <v>8:38:44</v>
+        <v>17:50:11</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>vatsal</v>
+        <v>parth</v>
       </c>
       <c r="B26" t="str">
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C26" s="1">
-        <v>45416.84626157407</v>
+        <v>45413.74621527778</v>
       </c>
       <c r="D26" t="str">
-        <v>14:9:6</v>
+        <v>17:52:23</v>
       </c>
       <c r="E26" t="str">
-        <v>20:18:15</v>
+        <v>17:54:17</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>vatsal</v>
+        <v>parth</v>
       </c>
       <c r="B27" t="str">
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C27" s="1">
-        <v>45416.846269837966</v>
+        <v>45413.75671296296</v>
       </c>
       <c r="D27" t="str">
-        <v>14:9:6</v>
+        <v>17:54:23</v>
       </c>
       <c r="E27" t="str">
-        <v>20:18:15</v>
+        <v>18:7:23</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>avi</v>
+        <v>parth</v>
       </c>
       <c r="B28" t="str">
-        <v>avi@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C28" s="1">
-        <v>45416.360501296294</v>
+        <v>45414.39465277778</v>
       </c>
       <c r="D28" t="str">
-        <v>8:37:40</v>
+        <v>9:27:54</v>
       </c>
       <c r="E28" t="str">
-        <v>8:38:44</v>
+        <v>9:28:5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>test</v>
+        <v>parth</v>
       </c>
       <c r="B29" t="str">
-        <v>test@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C29" s="1">
-        <v>45415.51063256944</v>
+        <v>45414.39488425926</v>
       </c>
       <c r="D29" t="str">
-        <v>12:5:48</v>
+        <v>9:28:8</v>
       </c>
       <c r="E29" t="str">
-        <v>12:15:2</v>
+        <v>9:28:25</v>
       </c>
     </row>
     <row r="30">
@@ -904,7 +904,7 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C30" s="1">
-        <v>45414.399427777775</v>
+        <v>45414.39942129629</v>
       </c>
       <c r="D30" t="str">
         <v>9:34:34</v>
@@ -915,104 +915,104 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>parth</v>
+        <v>test</v>
       </c>
       <c r="B31" t="str">
-        <v>parthpatel082828@gmail.com</v>
+        <v>test@gmail.com</v>
       </c>
       <c r="C31" s="1">
-        <v>45414.39488688658</v>
+        <v>45415.510625</v>
       </c>
       <c r="D31" t="str">
-        <v>9:28:8</v>
+        <v>12:5:48</v>
       </c>
       <c r="E31" t="str">
-        <v>9:28:25</v>
+        <v>12:15:2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>parth</v>
+        <v>avi</v>
       </c>
       <c r="B32" t="str">
-        <v>parthpatel082828@gmail.com</v>
+        <v>avi@gmail.com</v>
       </c>
       <c r="C32" s="1">
-        <v>45414.39466230324</v>
+        <v>45416.360497685186</v>
       </c>
       <c r="D32" t="str">
-        <v>9:27:54</v>
+        <v>8:37:40</v>
       </c>
       <c r="E32" t="str">
-        <v>9:28:5</v>
+        <v>8:38:44</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>parth</v>
+        <v>vatsal</v>
       </c>
       <c r="B33" t="str">
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C33" s="1">
-        <v>45413.75671300926</v>
+        <v>45416.84626157407</v>
       </c>
       <c r="D33" t="str">
-        <v>17:54:23</v>
+        <v>14:9:6</v>
       </c>
       <c r="E33" t="str">
-        <v>18:7:23</v>
+        <v>20:18:15</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>parth</v>
+        <v>vatsal</v>
       </c>
       <c r="B34" t="str">
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C34" s="1">
-        <v>45413.74621600694</v>
+        <v>45416.846269837966</v>
       </c>
       <c r="D34" t="str">
-        <v>17:52:23</v>
+        <v>14:9:6</v>
       </c>
       <c r="E34" t="str">
-        <v>17:54:17</v>
+        <v>20:18:15</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>parth</v>
+        <v>avi</v>
       </c>
       <c r="B35" t="str">
-        <v>parthpatel082828@gmail.com</v>
+        <v>avi@gmail.com</v>
       </c>
       <c r="C35" s="1">
-        <v>45411.74335091435</v>
+        <v>45416.360501296294</v>
       </c>
       <c r="D35" t="str">
-        <v>17:2:6</v>
+        <v>8:37:40</v>
       </c>
       <c r="E35" t="str">
-        <v>17:50:11</v>
+        <v>8:38:44</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>parth</v>
+        <v>test</v>
       </c>
       <c r="B36" t="str">
-        <v>parthpatel082828@gmail.com</v>
+        <v>test@gmail.com</v>
       </c>
       <c r="C36" s="1">
-        <v>45411.70991153935</v>
+        <v>45415.51063256944</v>
       </c>
       <c r="D36" t="str">
-        <v>17:1:31</v>
+        <v>12:5:48</v>
       </c>
       <c r="E36" t="str">
-        <v>17:1:57</v>
+        <v>12:15:2</v>
       </c>
     </row>
     <row r="37">
@@ -1023,30 +1023,30 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C37" s="1">
-        <v>45406.67672707176</v>
+        <v>45414.399427777775</v>
       </c>
       <c r="D37" t="str">
-        <v>15:52:4</v>
+        <v>9:34:34</v>
       </c>
       <c r="E37" t="str">
-        <v>16:12:36</v>
+        <v>9:34:41</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Jignesh</v>
+        <v>parth</v>
       </c>
       <c r="B38" t="str">
-        <v>jignesh1234@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C38" s="1">
-        <v>45390.771060914354</v>
+        <v>45414.39488688658</v>
       </c>
       <c r="D38" t="str">
-        <v>18:29:2</v>
+        <v>9:28:8</v>
       </c>
       <c r="E38" t="str">
-        <v>18:30:5</v>
+        <v>9:28:25</v>
       </c>
     </row>
     <row r="39">
@@ -1057,30 +1057,30 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C39" s="1">
-        <v>45390.77028099537</v>
+        <v>45414.39466230324</v>
       </c>
       <c r="D39" t="str">
-        <v>18:27:0</v>
+        <v>9:27:54</v>
       </c>
       <c r="E39" t="str">
-        <v>18:28:23</v>
+        <v>9:28:5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Jignesh</v>
+        <v>parth</v>
       </c>
       <c r="B40" t="str">
-        <v>jignesh1234@gmail.com</v>
+        <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C40" s="1">
-        <v>45390.76887056713</v>
+        <v>45413.75671300926</v>
       </c>
       <c r="D40" t="str">
-        <v>18:26:42</v>
+        <v>17:54:23</v>
       </c>
       <c r="E40" t="str">
-        <v>18:26:49</v>
+        <v>18:7:23</v>
       </c>
     </row>
     <row r="41">
@@ -1091,18 +1091,137 @@
         <v>parthpatel082828@gmail.com</v>
       </c>
       <c r="C41" s="1">
+        <v>45413.74621600694</v>
+      </c>
+      <c r="D41" t="str">
+        <v>17:52:23</v>
+      </c>
+      <c r="E41" t="str">
+        <v>17:54:17</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B42" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C42" s="1">
+        <v>45411.74335091435</v>
+      </c>
+      <c r="D42" t="str">
+        <v>17:2:6</v>
+      </c>
+      <c r="E42" t="str">
+        <v>17:50:11</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B43" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C43" s="1">
+        <v>45411.70991153935</v>
+      </c>
+      <c r="D43" t="str">
+        <v>17:1:31</v>
+      </c>
+      <c r="E43" t="str">
+        <v>17:1:57</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B44" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C44" s="1">
+        <v>45406.67672707176</v>
+      </c>
+      <c r="D44" t="str">
+        <v>15:52:4</v>
+      </c>
+      <c r="E44" t="str">
+        <v>16:12:36</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Jignesh</v>
+      </c>
+      <c r="B45" t="str">
+        <v>jignesh1234@gmail.com</v>
+      </c>
+      <c r="C45" s="1">
+        <v>45390.771060914354</v>
+      </c>
+      <c r="D45" t="str">
+        <v>18:29:2</v>
+      </c>
+      <c r="E45" t="str">
+        <v>18:30:5</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B46" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C46" s="1">
+        <v>45390.77028099537</v>
+      </c>
+      <c r="D46" t="str">
+        <v>18:27:0</v>
+      </c>
+      <c r="E46" t="str">
+        <v>18:28:23</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Jignesh</v>
+      </c>
+      <c r="B47" t="str">
+        <v>jignesh1234@gmail.com</v>
+      </c>
+      <c r="C47" s="1">
+        <v>45390.76887056713</v>
+      </c>
+      <c r="D47" t="str">
+        <v>18:26:42</v>
+      </c>
+      <c r="E47" t="str">
+        <v>18:26:49</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>parth</v>
+      </c>
+      <c r="B48" t="str">
+        <v>parthpatel082828@gmail.com</v>
+      </c>
+      <c r="C48" s="1">
         <v>45387.22928240741</v>
       </c>
-      <c r="D41" t="str">
+      <c r="D48" t="str">
         <v>02:53 PM</v>
       </c>
-      <c r="E41" t="str">
+      <c r="E48" t="str">
         <v>02:54 PM</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E48"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>